<commit_message>
refine the sematic rules
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Compiler-Semantic-Analyzer\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FDAE356-CDA6-48CE-A5B3-FCE59A8491A4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F40888-FC00-4A08-B1D9-EA14897F6FBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
   <si>
     <t>S</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>&lt;AssignStmt&gt;</t>
-  </si>
-  <si>
-    <t>return &lt;Exprsn&gt; ;</t>
   </si>
   <si>
     <t>while ( &lt;Exprsn&gt; ) &lt;StmtBlock&gt;</t>
@@ -217,12 +214,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ID not in var table : ERROR
-else: &lt;Factor&gt;.val = ID.name
-&lt;Factor&gt;.valType = 'var'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;Item&gt;.val = &lt;Factor&gt;.val
 &lt;Item&gt;.valType = &lt;Factor&gt;.valType</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -235,34 +226,6 @@
   <si>
     <t>&lt;E&gt;.val = &lt;A&gt;.val
 &lt;E&gt;.valType = &lt;A&gt;.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>newTemp.valType = calc(&lt;F&gt;, &lt;I2&gt;)
-IR = 'newTemp = &lt;F&gt;.val / &lt;I2&gt;.val'
-&lt;I1&gt;.val = newTemp
-&lt;I1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>newTemp.valType = calc(&lt;F&gt;, &lt;I2&gt;)
-IR = 'newTemp = &lt;F&gt;.val * &lt;I2&gt;.val'
-&lt;I1&gt;.val = newTemp
-&lt;I1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>newTemp.valType = calc(&lt;I&gt;, &lt;A2&gt;)
-IR = 'newTemp = &lt;I&gt;.val - &lt;A2&gt;.val'
-&lt;A1&gt;.val = newTemp
-&lt;A1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>newTemp.valType = calc(&lt;I&gt;, &lt;A2&gt;)
-IR = 'newTemp = &lt;I&gt;.val + &lt;A2&gt;.val'
-&lt;A1&gt;.val = newTemp
-&lt;A1&gt;.valType = newTemp.valType</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -339,21 +302,7 @@
   </si>
   <si>
     <t xml:space="preserve">ID.valType = 'float'
-if &lt;E&gt;.valType is not 'float': transType
-IR = 'ID = &lt;E&gt;.val'
-insert into var symbol table </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ID.valType = 'float'
 IR = 'ID = 0.0'
-insert into var symbol table </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ID.valType = 'int'
-if &lt;E&gt;.valType is not 'int': transType
-IR = 'ID = &lt;E&gt;.val'
 insert into var symbol table </t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -374,35 +323,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>ID not in func table: ERROR 
-&lt;FC&gt;.args does not match func table item: ERROR
-if need to transfer type for args: transType
-IR = 'newTemp = call ID(...)'
-newTemp.valType = ID.funcReturnType
-&lt;F&gt;.val = newTemp
-&lt;F&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>return &lt;Exprsn&gt; ;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'ret ;'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'ret &lt;E&gt;.val ;'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ID = &lt;Exprsn&gt; ;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if ID not in var table: ERROR
-if ID and &lt;E&gt; valType not match: transType
-IR = 'ID = &lt;E&gt;.val'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -463,43 +384,11 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;S&gt;.IR = &lt;AS&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;S&gt;.IR = &lt;VD&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;S&gt;.IR = &lt;IS&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;S&gt;.IR = &lt;WS&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;S&gt;.IR = &lt;RS&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;Stmt&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Stmts1&gt;.IR = &lt;S&gt;.IR + &lt;Stmts2&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>{ &lt;Stmts&gt; }</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -556,6 +445,151 @@
   <si>
     <t>S'.IR = S.IR
 print(S'.IR)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ID.valType = 'int'
+if &lt;E&gt;.valType is not 'int': ERROR
+IR = 'ID = &lt;E&gt;.val'
+insert into var symbol table </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ID.valType = 'float'
+if &lt;E&gt;.valType is not 'float': ERROR
+IR = 'ID = &lt;E&gt;.val'
+insert into var symbol table </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if ID not in var table: ERROR
+if ID and &lt;E&gt; valType not match: ERROR
+IR = 'ID = &lt;E&gt;.val'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;I&gt; &lt;A2&gt; type not match: ERROR
+IR = 'newTemp = &lt;I&gt;.val + &lt;A2&gt;.val'
+&lt;A1&gt;.val = newTemp
+&lt;A1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;I&gt; &lt;A2&gt; type not match: ERROR
+IR = 'newTemp = &lt;I&gt;.val - &lt;A2&gt;.val'
+&lt;A1&gt;.val = newTemp
+&lt;A1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID not in func table: ERROR 
+&lt;FC&gt;.args does not match func table item: ERROR
+if type of args don't match: ERROR
+IR = 'newTemp = call ID(...)'
+newTemp.valType = ID.funcReturnType
+&lt;F&gt;.val = newTemp
+&lt;F&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID not in var table : ERROR
+else: &lt;Factor&gt;.val = ID.name
+&lt;Factor&gt;.valType = ID.varType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;F&gt; &lt;I2&gt; type don't match: ERROR
+IR = 'newTemp = &lt;F&gt;.val / &lt;I2&gt;.val'
+&lt;I1&gt;.val = newTemp
+&lt;I1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;F&gt; &lt;I2&gt; type don't match: ERROR
+IR = 'newTemp = &lt;F&gt;.val * &lt;I2&gt;.val'
+&lt;I1&gt;.val = newTemp
+&lt;I1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>return &lt;Exprsn&gt; ;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>return ;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;AS&gt;.IR
+&lt;S&gt;.returnType = 'void'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IR = 'ret &lt;E&gt;.val ;'
+&lt;RS&gt;.returnType = &lt;E&gt;.varType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>IR = 'ret ;'
+&lt;RS&gt;.returnType = 'void'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;RS&gt;.IR
+&lt;S&gt;.returnType = &lt;RS&gt;.returnType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;VD&gt;.IR
+&lt;S&gt;.returnType = 'void'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR
+&lt;Stmts&gt;.returnType = &lt;S&gt;.returnType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
+&lt;SB&gt;.returnType = &lt;S&gt;.returnType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;IS&gt;.IR
+&lt;S&gt;.returnType = &lt;IS&gt;.returnType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;WS&gt;.IR
+&lt;S&gt;.returnType = &lt;WS&gt;.returnType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
+if &lt;S&gt; &lt;Stmts2&gt; rT equal: &lt;Stmts1&gt;.rT = &lt;Stmt&gt;.rT
+else: ERROR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;SB1&gt;.rT equals to &lt;SB2&gt;.rT: &lt;IS&gt;.rT = &lt;SB1&gt;.rT
+else: ERROR
+&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' 
++ &lt;SB1&gt;.IR + 'goto L2' 
++ 'L1:' + &lt;SB2&gt;.IR 
++ 'L2:'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;WS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;WS&gt;.IR = 'L1:' + &lt;E&gt;.IR 
++ 'if(&lt;E&gt;.val != 1) goto L2:'
++ &lt;SB&gt;.IR + 'goto L1' 
++ 'L2:'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -591,7 +625,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -608,7 +642,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -621,8 +655,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -943,8 +980,8 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -957,24 +994,24 @@
   <sheetData>
     <row r="1" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -985,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -996,7 +1033,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1007,7 +1044,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1015,10 +1052,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1029,7 +1066,7 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1040,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>78</v>
+        <v>98</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1048,10 +1085,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1062,7 +1099,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1073,7 +1110,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1084,7 +1121,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1095,7 +1132,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1106,7 +1143,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1117,7 +1154,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1125,10 +1162,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1139,7 +1176,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>92</v>
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1150,7 +1187,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1161,7 +1198,7 @@
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1172,7 +1209,7 @@
         <v>19</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1180,21 +1217,21 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>106</v>
+      <c r="C22" s="3" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1202,10 +1239,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>105</v>
+        <v>86</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1215,8 +1252,8 @@
       <c r="B24" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>100</v>
+      <c r="C24" s="3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1226,8 +1263,8 @@
       <c r="B25" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="2" t="s">
-        <v>101</v>
+      <c r="C25" s="3" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1237,8 +1274,8 @@
       <c r="B26" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>102</v>
+      <c r="C26" s="3" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1248,8 +1285,8 @@
       <c r="B27" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>103</v>
+      <c r="C27" s="3" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1257,10 +1294,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1268,10 +1305,10 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1279,10 +1316,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1290,26 +1327,32 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>83</v>
+        <v>108</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1317,271 +1360,274 @@
         <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="C35" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="153" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>69</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="73.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="C45" s="3" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>66</v>
+        <v>105</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>46</v>
-      </c>
       <c r="C48" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="49" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>62</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="114" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="C53" s="3" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="1" t="s">
-        <v>54</v>
-      </c>
       <c r="C54" s="3" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="55" spans="1:3" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B57" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B57" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="C57" s="3" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add details for var symbol table
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Compiler-Semantic-Analyzer\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4F40888-FC00-4A08-B1D9-EA14897F6FBF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746214E2-7086-4275-B500-AFD3FEB79DA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="123">
   <si>
     <t>S</t>
   </si>
@@ -392,33 +392,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>check the return statement in SB (may need to transType)
-&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'float'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>check the return statement in SB (may need to transType)
-&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'int'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>check the return statement in SB (may need to transType)
-&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'void'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;FuncDecl&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -540,21 +513,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;S&gt;.IR = &lt;VD&gt;.IR
-&lt;S&gt;.returnType = 'void'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR
-&lt;Stmts&gt;.returnType = &lt;S&gt;.returnType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
-&lt;SB&gt;.returnType = &lt;S&gt;.returnType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;S&gt;.IR = &lt;IS&gt;.IR
 &lt;S&gt;.returnType = &lt;IS&gt;.returnType</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -562,17 +520,6 @@
   <si>
     <t>&lt;S&gt;.IR = &lt;WS&gt;.IR
 &lt;S&gt;.returnType = &lt;WS&gt;.returnType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
-if &lt;S&gt; &lt;Stmts2&gt; rT equal: &lt;Stmts1&gt;.rT = &lt;Stmt&gt;.rT
-else: ERROR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
-&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -585,11 +532,77 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
+    <t>&lt;VarDecl&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;VD&gt;.IR
+&lt;S&gt;.returnType = 'void'
+&lt;Stmt&gt;.varAmount += 1 (default is 0)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR
+&lt;Stmts&gt;.returnType = &lt;S&gt;.returnType
+&lt;Stmts&gt;.varAmount = &lt;Stmt&gt;.varAmount</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
+if &lt;S&gt; &lt;Stmts2&gt; rT equal: &lt;Stmts1&gt;.rT = &lt;Stmt&gt;.rT
+else: ERROR
+&lt;Stmts1&gt;.varAmount = &lt;Stmt&gt;vA + &lt;Stmts2&gt;.vA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
+&lt;SB&gt;.returnType = &lt;S&gt;.returnType
+&lt;SB&gt;.varAmount = &lt;S&gt;.vA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check the return statement in SB (may need to transType)
+&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'int'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table
+push &lt;SB&gt;.varAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check the return statement in SB (may need to transType)
+&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'float'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table
+push &lt;SB&gt;.varAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>check the return statement in SB (may need to transType)
+&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'void'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table
+push &lt;SB&gt;.varAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve"> &lt;WS&gt;.returnType = &lt;SB&gt;.returnType
 &lt;WS&gt;.IR = 'L1:' + &lt;E&gt;.IR 
 + 'if(&lt;E&gt;.val != 1) goto L2:'
 + &lt;SB&gt;.IR + 'goto L1' 
-+ 'L2:'</t>
++ 'L2:'
+push &lt;SB&gt;.varAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'
+push &lt;SB&gt;.varAmount vars from var symbol table</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -616,18 +629,12 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -642,7 +649,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -656,9 +663,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -980,8 +984,8 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1000,7 +1004,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1011,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1022,7 +1026,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1033,7 +1037,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1044,7 +1048,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1052,10 +1056,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1077,7 +1081,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1099,10 +1103,10 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1110,10 +1114,10 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>5</v>
       </c>
@@ -1121,10 +1125,10 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="100.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
@@ -1132,7 +1136,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>90</v>
+        <v>120</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1220,7 +1224,7 @@
         <v>87</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,7 +1235,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1242,7 +1246,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1250,10 +1254,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>4</v>
+        <v>113</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1264,7 +1268,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1275,7 +1279,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1286,7 +1290,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1297,7 +1301,7 @@
         <v>85</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1308,7 +1312,7 @@
         <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1316,10 +1320,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>107</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1327,20 +1331,20 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="C31" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:3" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="4" t="s">
         <v>121</v>
       </c>
     </row>
@@ -1352,10 +1356,10 @@
         <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="61.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>24</v>
       </c>
@@ -1363,7 +1367,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1451,7 +1455,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="72.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1462,7 +1466,7 @@
         <v>40</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1484,7 +1488,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1495,7 +1499,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1550,7 +1554,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="114" customHeight="1" x14ac:dyDescent="0.2">
@@ -1561,7 +1565,7 @@
         <v>49</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
add Node class when doing semantic analysis
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Compiler-Semantic-Analyzer\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746214E2-7086-4275-B500-AFD3FEB79DA6}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CFB30A8-C24F-4411-A620-A9D0A0E50182}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="90" windowWidth="16335" windowHeight="10830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -536,74 +536,65 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;S&gt;.IR = &lt;VD&gt;.IR
-&lt;S&gt;.returnType = 'void'
-&lt;Stmt&gt;.varAmount += 1 (default is 0)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR
-&lt;Stmts&gt;.returnType = &lt;S&gt;.returnType
-&lt;Stmts&gt;.varAmount = &lt;Stmt&gt;.varAmount</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
+&lt;SB&gt;.returnType = &lt;S&gt;.returnType
+&lt;SB&gt;.innerVarAmount = &lt;S&gt;.vA</t>
   </si>
   <si>
     <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
 if &lt;S&gt; &lt;Stmts2&gt; rT equal: &lt;Stmts1&gt;.rT = &lt;Stmt&gt;.rT
 else: ERROR
-&lt;Stmts1&gt;.varAmount = &lt;Stmt&gt;vA + &lt;Stmts2&gt;.vA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
-&lt;SB&gt;.returnType = &lt;S&gt;.returnType
-&lt;SB&gt;.varAmount = &lt;S&gt;.vA</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>check the return statement in SB (may need to transType)
+&lt;Stmts1&gt;.innerVarAmount = &lt;Stmt&gt;vA + &lt;Stmts2&gt;.vA</t>
+  </si>
+  <si>
+    <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR
+&lt;Stmts&gt;.returnType = &lt;S&gt;.returnType
+&lt;Stmts&gt;.innerVarAmount = &lt;Stmt&gt;.innerVarAmount</t>
+  </si>
+  <si>
+    <t>&lt;S&gt;.IR = &lt;VD&gt;.IR
+&lt;S&gt;.returnType = 'void'
+&lt;Stmt&gt;.innerVarAmount += 1 (default is 0)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;WS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;WS&gt;.IR = 'L1:' + &lt;E&gt;.IR 
++ 'if(&lt;E&gt;.val != 1) goto L2:'
++ &lt;SB&gt;.IR + 'goto L1' 
++ 'L2:'
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
 &lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
 &lt;FD&gt;.returnType = 'int'
 &lt;FD&gt;.paramName = &lt;FP&gt;.paramName
 &lt;FD&gt;.paramType = &lt;FP&gt;.paramType
 insert into func symbol table
-push &lt;SB&gt;.varAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>check the return statement in SB (may need to transType)
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
 &lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
 &lt;FD&gt;.returnType = 'float'
 &lt;FD&gt;.paramName = &lt;FP&gt;.paramName
 &lt;FD&gt;.paramType = &lt;FP&gt;.paramType
 insert into func symbol table
-push &lt;SB&gt;.varAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>check the return statement in SB (may need to transType)
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
 &lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
 &lt;FD&gt;.returnType = 'void'
 &lt;FD&gt;.paramName = &lt;FP&gt;.paramName
 &lt;FD&gt;.paramType = &lt;FP&gt;.paramType
 insert into func symbol table
-push &lt;SB&gt;.varAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;WS&gt;.returnType = &lt;SB&gt;.returnType
-&lt;WS&gt;.IR = 'L1:' + &lt;E&gt;.IR 
-+ 'if(&lt;E&gt;.val != 1) goto L2:'
-+ &lt;SB&gt;.IR + 'goto L1' 
-+ 'L2:'
-push &lt;SB&gt;.varAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
-&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'
-push &lt;SB&gt;.varAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
   </si>
 </sst>
 </file>
@@ -984,8 +975,8 @@
   </sheetPr>
   <dimension ref="A1:C58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD35"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="A1:C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1114,7 +1105,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1125,7 +1116,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1136,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1224,7 +1215,7 @@
         <v>87</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -1235,7 +1226,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1246,7 +1237,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1257,7 +1248,7 @@
         <v>113</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1345,7 +1336,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1367,7 +1358,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="51" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
rewrite function deepCopy of recursive copy array and object
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jake/Git/Compiler-Semantic-Analyzer/Assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7ECEBFF-AB91-9F40-84D3-F11209ACF0E7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A521E2-C6CC-1E4F-8994-8D5E769A0604}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A Test Sheet" sheetId="1" r:id="rId1"/>
@@ -337,13 +337,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;Arg1&gt;.args = &lt;Arg2&gt;.params
-&lt;Arg1&gt;.argType = &lt;Arg2&gt;.paramType
-&lt;Arg1&gt;.args.putHead(&lt;E&gt;.val)
-&lt;Arg1&gt;.argType.putHead(&lt;E&gt;.valType)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;Arg&gt;.args.putHead(&lt;E&gt;.val)
 &lt;Arg&gt;.argType.putHead(&lt;E&gt;.valType)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -595,6 +588,13 @@
 &lt;FD&gt;.paramType = &lt;FP&gt;.paramType
 insert into func symbol table
 push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+  </si>
+  <si>
+    <t>&lt;Arg1&gt;.args = &lt;Arg2&gt;.args
+&lt;Arg1&gt;.argType = &lt;Arg2&gt;.argType
+&lt;Arg1&gt;.args.putHead(&lt;E&gt;.val)
+&lt;Arg1&gt;.argType.putHead(&lt;E&gt;.valType)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -976,7 +976,7 @@
   <dimension ref="A1:C58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+      <selection activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
@@ -995,7 +995,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="51" customHeight="1">
@@ -1006,7 +1006,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="51" customHeight="1">
@@ -1017,7 +1017,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="51" customHeight="1">
@@ -1028,7 +1028,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="51" customHeight="1">
@@ -1039,7 +1039,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="51" customHeight="1">
@@ -1047,10 +1047,10 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="51" customHeight="1">
@@ -1072,7 +1072,7 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="51" customHeight="1">
@@ -1094,7 +1094,7 @@
         <v>8</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="124.5" customHeight="1">
@@ -1105,7 +1105,7 @@
         <v>9</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="124.5" customHeight="1">
@@ -1116,7 +1116,7 @@
         <v>10</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="124.5" customHeight="1">
@@ -1127,7 +1127,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="51" customHeight="1">
@@ -1138,7 +1138,7 @@
         <v>13</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="51" customHeight="1">
@@ -1149,7 +1149,7 @@
         <v>14</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="51" customHeight="1">
@@ -1157,10 +1157,10 @@
         <v>12</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="51" customHeight="1">
@@ -1171,7 +1171,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="70.5" customHeight="1">
@@ -1182,7 +1182,7 @@
         <v>17</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="51" customHeight="1">
@@ -1212,10 +1212,10 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="72" customHeight="1">
@@ -1226,7 +1226,7 @@
         <v>22</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="51" customHeight="1">
@@ -1234,10 +1234,10 @@
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="51" customHeight="1">
@@ -1245,10 +1245,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="51" customHeight="1">
@@ -1259,7 +1259,7 @@
         <v>24</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="51" customHeight="1">
@@ -1270,7 +1270,7 @@
         <v>25</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="51" customHeight="1">
@@ -1281,7 +1281,7 @@
         <v>26</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="51" customHeight="1">
@@ -1289,10 +1289,10 @@
         <v>23</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="58.5" customHeight="1">
@@ -1303,7 +1303,7 @@
         <v>74</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="51" customHeight="1">
@@ -1311,10 +1311,10 @@
         <v>26</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="51" customHeight="1">
@@ -1322,10 +1322,10 @@
         <v>26</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="93" customHeight="1">
@@ -1336,7 +1336,7 @@
         <v>28</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="118.5" customHeight="1">
@@ -1347,7 +1347,7 @@
         <v>29</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="61.5" customHeight="1">
@@ -1358,7 +1358,7 @@
         <v>30</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="51" customHeight="1">
@@ -1446,7 +1446,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="72.75" customHeight="1">
@@ -1457,7 +1457,7 @@
         <v>40</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="51" customHeight="1">
@@ -1479,7 +1479,7 @@
         <v>42</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="68.25" customHeight="1">
@@ -1490,7 +1490,7 @@
         <v>43</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="51" customHeight="1">
@@ -1545,7 +1545,7 @@
         <v>48</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="114" customHeight="1">
@@ -1556,7 +1556,7 @@
         <v>49</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="51" customHeight="1">
@@ -1589,7 +1589,7 @@
         <v>14</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="56" spans="1:3" ht="51" customHeight="1">
@@ -1600,7 +1600,7 @@
         <v>15</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="57" spans="1:3" ht="64.5" customHeight="1">
@@ -1611,7 +1611,7 @@
         <v>54</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>77</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:3" ht="51" customHeight="1">
@@ -1622,7 +1622,7 @@
         <v>31</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add some semantic analysis functions
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jake/Git/Compiler-Semantic-Analyzer/Assignments/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Compiler-Semantic-Analyzer\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5A18C31-D1E6-3A47-BE24-9A3F76C5F3D3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4872272A-274C-487D-9F29-C84A8A2A192E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A Test Sheet" sheetId="1" r:id="rId1"/>
@@ -209,148 +209,7 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;Factor&gt;.val = &lt;Exprsn&gt;.val
-&lt;Factor&gt;.valType = &lt;Exprsn&gt;.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Item&gt;.val = &lt;Factor&gt;.val
-&lt;Item&gt;.valType = &lt;Factor&gt;.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;A&gt;.val = &lt;Item&gt;.val
-&lt;A&gt;.valType = &lt;Item&gt;.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;E&gt;.val = &lt;A&gt;.val
-&lt;E&gt;.valType = &lt;A&gt;.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'newTemp1 = (&lt;A&gt;.val != &lt;E2&gt;.val); 
-if newTemp1 goto L1 
-newTemp2 = 0
-goto L2
-L1: newTemp2 = 1
-L2:'
-newTemp.valType = 'int'
-&lt;E1&gt;.val = newTemp
-&lt;E1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'newTemp1 = (&lt;A&gt;.val == &lt;E2&gt;.val); 
-if newTemp1 goto L1 
-newTemp2 = 0
-goto L2
-L1: newTemp2 = 1
-L2:'
-newTemp.valType = 'int'
-&lt;E1&gt;.val = newTemp
-&lt;E1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'newTemp1 = (&lt;A&gt;.val &gt;= &lt;E2&gt;.val); 
-if newTemp1 goto L1 
-newTemp2 = 0
-goto L2
-L1: newTemp2 = 1
-L2:'
-newTemp.valType = 'int'
-&lt;E1&gt;.val = newTemp
-&lt;E1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'newTemp1 = (&lt;A&gt;.val &gt; &lt;E2&gt;.val); 
-if newTemp1 goto L1 
-newTemp2 = 0
-goto L2
-L1: newTemp2 = 1
-L2:'
-newTemp.valType = 'int'
-&lt;E1&gt;.val = newTemp
-&lt;E1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'newTemp1 = (&lt;A&gt;.val &lt;= &lt;E2&gt;.val); 
-if newTemp1 goto L1 
-newTemp2 = 0
-goto L2
-L1: newTemp2 = 1
-L2:'
-newTemp.valType = 'int'
-&lt;E1&gt;.val = newTemp
-&lt;E1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'newTemp1 = (&lt;A&gt;.val &lt; &lt;E2&gt;.val); 
-if newTemp1 goto L1 
-newTemp2 = 0
-goto L2
-L1: newTemp2 = 1
-L2:'
-newTemp.valType = 'int'
-&lt;E1&gt;.val = newTemp
-&lt;E1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ID.valType = 'float'
-IR = 'ID = 0.0'
-insert into var symbol table </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ID.valType = 'int'
-IR = 'ID = 0'
-insert into var symbol table </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Ac&gt;.args = &lt;Arg&gt;.args
-&lt;Ac&gt;.argType = &lt;Arg&gt;.argType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;F&gt;.args = &lt;Ac&gt;.args
-&lt;F&gt;.argType = &lt;Ac&gt;.argType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>ID = &lt;Exprsn&gt; ;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;P&gt;.type = 'int'
-&lt;P&gt;.name = ID.name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;P&gt;.type = 'float'
-&lt;P&gt;.name = ID.name</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;Arg&gt;.args.putHead(&lt;E&gt;.val)
-&lt;Arg&gt;.argType.putHead(&lt;E&gt;.valType)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;PL&gt;.paramType.putHead(&lt;P&gt;.type)
-&lt;PL&gt;.paramName.putHead(&lt;P&gt;.name)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;PL1&gt;.paramType = &lt;PL2&gt;.paramType
-&lt;PL1&gt;.paramName = &lt;PL2&gt;.paramName
-&lt;PL1&gt;.paramType.putHead(&lt;P&gt;.type)
-&lt;PL1&gt;.paramName.putHead(&lt;P&gt;.name)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -368,11 +227,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;FP&gt;.paramType = &lt;PL&gt;.paramType 
-&lt;FP&gt;.paramName = &lt;PL&gt;.paramName</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;AssignStmt&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -414,70 +268,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">ID.valType = 'int'
-if &lt;E&gt;.valType is not 'int': ERROR
-IR = 'ID = &lt;E&gt;.val'
-insert into var symbol table </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">ID.valType = 'float'
-if &lt;E&gt;.valType is not 'float': ERROR
-IR = 'ID = &lt;E&gt;.val'
-insert into var symbol table </t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if ID not in var table: ERROR
-if ID and &lt;E&gt; valType not match: ERROR
-IR = 'ID = &lt;E&gt;.val'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if &lt;I&gt; &lt;A2&gt; type not match: ERROR
-IR = 'newTemp = &lt;I&gt;.val + &lt;A2&gt;.val'
-&lt;A1&gt;.val = newTemp
-&lt;A1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if &lt;I&gt; &lt;A2&gt; type not match: ERROR
-IR = 'newTemp = &lt;I&gt;.val - &lt;A2&gt;.val'
-&lt;A1&gt;.val = newTemp
-&lt;A1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID not in func table: ERROR 
-&lt;FC&gt;.args does not match func table item: ERROR
-if type of args don't match: ERROR
-IR = 'newTemp = call ID(...)'
-newTemp.valType = ID.funcReturnType
-&lt;F&gt;.val = newTemp
-&lt;F&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID not in var table : ERROR
-else: &lt;Factor&gt;.val = ID.name
-&lt;Factor&gt;.valType = ID.varType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if &lt;F&gt; &lt;I2&gt; type don't match: ERROR
-IR = 'newTemp = &lt;F&gt;.val / &lt;I2&gt;.val'
-&lt;I1&gt;.val = newTemp
-&lt;I1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>if &lt;F&gt; &lt;I2&gt; type don't match: ERROR
-IR = 'newTemp = &lt;F&gt;.val * &lt;I2&gt;.val'
-&lt;I1&gt;.val = newTemp
-&lt;I1&gt;.valType = newTemp.valType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>return &lt;Exprsn&gt; ;</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -488,16 +278,6 @@
   <si>
     <t>&lt;S&gt;.IR = &lt;AS&gt;.IR
 &lt;S&gt;.returnType = 'void'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'ret &lt;E&gt;.val ;'
-&lt;RS&gt;.returnType = &lt;E&gt;.varType</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>IR = 'ret ;'
-&lt;RS&gt;.returnType = 'void'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -558,42 +338,304 @@
 push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
   </si>
   <si>
+    <t>&lt;Item&gt;.val = &lt;Factor&gt;.val
+&lt;Item&gt;.valType = &lt;Factor&gt;.valType
+&lt;Item&gt;.IR = &lt;Factor&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt;.val = &lt;Item&gt;.val
+&lt;A&gt;.valType = &lt;Item&gt;.valType
+&lt;A&gt;.IR = &lt;Item&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Arg&gt;.args.putHead(&lt;E&gt;.val)
+&lt;Arg&gt;.argType.putHead(&lt;E&gt;.valType)
+&lt;Arg&gt;.IR = &lt;E&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Arg1&gt;.args = &lt;Arg2&gt;.args
+&lt;Arg1&gt;.argType = &lt;Arg2&gt;.argType
+&lt;Arg1&gt;.args.putHead(&lt;E&gt;.val)
+&lt;Arg1&gt;.argType.putHead(&lt;E&gt;.valType)
+&lt;Arg1&gt;.IR = &lt;E&gt;.IR + &lt;Arg2&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Ac&gt;.args = &lt;Arg&gt;.args
+&lt;Ac&gt;.argType = &lt;Arg&gt;.argType
+&lt;Ac&gt;.IR = &lt;Arg&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;F&gt;.args = &lt;Ac&gt;.args
+&lt;F&gt;.argType = &lt;Ac&gt;.argType
+&lt;F&gt;.IR = &lt;Ac&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Factor&gt;.val = &lt;Exprsn&gt;.val
+&lt;Factor&gt;.valType = &lt;Exprsn&gt;.valType
+&lt;Factor&gt;.IR = &lt;Exprsn&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;F&gt; &lt;I2&gt; type don't match: ERROR
+&lt;I1&gt;.IR = &lt;F&gt;.IR + &lt;I2&gt;.IR
++ 'newTemp = &lt;F&gt;.val / &lt;I2&gt;.val'
+&lt;I1&gt;.val = newTemp
+&lt;I1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;F&gt; &lt;I2&gt; type don't match: ERROR
+&lt;I1&gt;.IR = &lt;F&gt;.IR + &lt;I2&gt;.IR
++ 'newTemp = &lt;F&gt;.val * &lt;I2&gt;.val'
+&lt;I1&gt;.val = newTemp
+&lt;I1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;I&gt; &lt;A2&gt; type not match: ERROR
+&lt;A1&gt;.IR = &lt;I&gt;.IR + &lt;A2&gt;.IR 
++ 'newTemp = &lt;I&gt;.val - &lt;A2&gt;.val'
+&lt;A1&gt;.val = newTemp
+&lt;A1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;I&gt; &lt;A2&gt; type not match: ERROR
+&lt;A1&gt;.IR = &lt;I&gt;.IR + &lt;A2&gt;.IR 
++ 'newTemp = &lt;I&gt;.val + &lt;A2&gt;.val'
+&lt;A1&gt;.val = newTemp
+&lt;A1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;E&gt;.val = &lt;A&gt;.val
+&lt;E&gt;.valType = &lt;A&gt;.valType
+&lt;E&gt;.IR = &lt;A&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
     <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
 &lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'
 push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;RS&gt;.IR = 'ret ;'
+&lt;RS&gt;.returnType = 'void'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;RS&gt;.IR = 'ret &lt;E&gt;.val ;'
+&lt;RS&gt;.returnType = &lt;E&gt;.varType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if ID not in var table: ERROR
+if ID and &lt;E&gt; valType not match: ERROR
+&lt;AS&gt;.IR = &lt;E&gt;.IR + 'ID = &lt;E&gt;.val'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;P&gt;.type = 'float'
+&lt;P&gt;.name = ID.name
+&lt;P&gt;.IR = 'float ID'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;P&gt;.type = 'int'
+&lt;P&gt;.name = ID.name
+&lt;P&gt;.IR = 'int ID'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;PL1&gt;.paramType = &lt;PL2&gt;.paramType
+&lt;PL1&gt;.paramName = &lt;PL2&gt;.paramName
+&lt;PL1&gt;.paramType.putHead(&lt;P&gt;.type)
+&lt;PL1&gt;.paramName.putHead(&lt;P&gt;.name)
+&lt;PL1&gt;.IR = &lt;P&gt;.IR + ', ' + &lt;PL2&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;PL&gt;.paramType.putHead(&lt;P&gt;.type)
+&lt;PL&gt;.paramName.putHead(&lt;P&gt;.name)
+&lt;PL&gt;.IR = &lt;P&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;FP&gt;.paramType = &lt;PL&gt;.paramType 
+&lt;FP&gt;.paramName = &lt;PL&gt;.paramName
+&lt;FP&gt;.IR = &lt;PL&gt;.IR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
-&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'void'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
+&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'float'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table
+push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
+&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
 &lt;FD&gt;.returnType = 'int'
 &lt;FD&gt;.paramName = &lt;FP&gt;.paramName
 &lt;FD&gt;.paramType = &lt;FP&gt;.paramType
 insert into func symbol table
 push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
-  </si>
-  <si>
-    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
-&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'float'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
-  </si>
-  <si>
-    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
-&lt;FD&gt;.IR = 'def func(...)' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'void'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
-  </si>
-  <si>
-    <t>&lt;Arg1&gt;.args = &lt;Arg2&gt;.args
-&lt;Arg1&gt;.argType = &lt;Arg2&gt;.argType
-&lt;Arg1&gt;.args.putHead(&lt;E&gt;.val)
-&lt;Arg1&gt;.argType.putHead(&lt;E&gt;.valType)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ID.valType = 'float'
+if &lt;E&gt;.valType is not 'float': ERROR
+&lt;VD&gt;.IR = &lt;E&gt;.IR + 'ID = &lt;E&gt;.val'
+insert into var symbol table </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ID.valType = 'float'
+&lt;VD&gt;.IR = 'ID = 0e+00'
+insert into var symbol table </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ID.valType = 'int'
+if &lt;E&gt;.valType is not 'int': ERROR
+&lt;VD&gt;.IR = &lt;E&gt;.IR + 'ID = &lt;E&gt;.val'
+insert into var symbol table </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">ID.valType = 'int'
+&lt;VD&gt;.IR = 'ID = 0'
+insert into var symbol table </t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ID not in func table: ERROR 
+&lt;FC&gt;.args does not match func table item: ERROR
+if type of args don't match: ERROR
+ID.funcReturnType is void: ERROR
+&lt;F&gt;.IR = &lt;FC&gt;.IR + 'newTemp = call ID(...)'
+newTemp.valType = ID.funcReturnType
+&lt;F&gt;.val = newTemp
+&lt;F&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ID not in var table : ERROR
+else: &lt;Factor&gt;.val = ID.val
+&lt;Factor&gt;.valType = ID.varType
+</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="10"/>
+        <rFont val="更纱黑体 SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>&lt;Factor&gt;.IR = 'ID = xxx'</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt; &lt;E1&gt; type not match: ERROR
+&lt;E1&gt;.IR = &lt;A&gt;.IR + &lt;E1&gt;.IR +  
+'newTemp1 = (&lt;A&gt;.val != &lt;E2&gt;.val); 
+if newTemp1 goto L1 else L2
+L1: newTemp2 = 1
+goto L3
+L2: newTemp2 = 0
+L3:'
+newTemp.valType = 'int'
+&lt;E1&gt;.val = newTemp
+&lt;E1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt; &lt;E1&gt; type not match: ERROR
+&lt;E1&gt;.IR = &lt;A&gt;.IR + &lt;E1&gt;.IR +
+ 'newTemp1 = (&lt;A&gt;.val == &lt;E2&gt;.val); 
+if newTemp1 goto L1 else L2
+L1: newTemp2 = 1
+goto L3
+L2: newTemp2 = 0
+L3:'newTemp.valType = 'int'
+&lt;E1&gt;.val = newTemp
+&lt;E1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt; &lt;E1&gt; type not match: ERROR
+&lt;E1&gt;.IR = &lt;A&gt;.IR + &lt;E1&gt;.IR + 
+ 'newTemp1 = (&lt;A&gt;.val &gt;= &lt;E2&gt;.val); 
+if newTemp1 goto L1 else L2
+L1: newTemp2 = 1
+goto L3
+L2: newTemp2 = 0
+L3:'newTemp.valType = 'int'
+&lt;E1&gt;.val = newTemp
+&lt;E1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt; &lt;E1&gt; type not match: ERROR
+&lt;E1&gt;.IR = &lt;A&gt;.IR + &lt;E1&gt;.IR + 
+ 'newTemp1 = (&lt;A&gt;.val &gt; &lt;E2&gt;.val); 
+if newTemp1 goto L1 else L2
+L1: newTemp2 = 1
+goto L3
+L2: newTemp2 = 0
+L3:'newTemp.valType = 'int'
+&lt;E1&gt;.val = newTemp
+&lt;E1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt; &lt;E1&gt; type not match: ERROR
+&lt;E1&gt;.IR = &lt;A&gt;.IR + &lt;E1&gt;.IR +
+ 'newTemp1 = (&lt;A&gt;.val &lt;= &lt;E2&gt;.val); 
+if newTemp1 goto L1 else L2
+L1: newTemp2 = 1
+goto L3
+L2: newTemp2 = 0
+L3:'newTemp.valType = 'int'
+&lt;E1&gt;.val = newTemp
+&lt;E1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;A&gt; &lt;E1&gt; type not match: ERROR
+&lt;E1&gt;.IR = &lt;A&gt;.IR + &lt;E1&gt;.IR +
+ 'newTemp1 = (&lt;A&gt;.val &lt; &lt;E2&gt;.val); 
+if newTemp1 goto L1 else L2
+L1: newTemp2 = 1
+goto L3
+L2: newTemp2 = 0
+L3:'newTemp.valType = 'int'
+&lt;E1&gt;.val = newTemp
+&lt;E1&gt;.valType = newTemp.valType</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -601,7 +643,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -617,6 +659,13 @@
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <name val="更纱黑体 SC"/>
+      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -975,20 +1024,20 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:A58"/>
+    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.5" style="2" customWidth="1"/>
-    <col min="4" max="4" width="48.1640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.1640625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51" customHeight="1">
+    <row r="1" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -999,10 +1048,10 @@
         <v>0</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="51" customHeight="1">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -1013,10 +1062,10 @@
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="51" customHeight="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -1027,10 +1076,10 @@
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="51" customHeight="1">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1041,10 +1090,10 @@
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="51" customHeight="1">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -1055,10 +1104,10 @@
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="51" customHeight="1">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -1066,13 +1115,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="51" customHeight="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -1083,10 +1132,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="64.5" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -1097,10 +1146,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" customHeight="1">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -1111,10 +1160,10 @@
         <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="74.25" customHeight="1">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -1125,10 +1174,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="124.5" customHeight="1">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -1139,10 +1188,10 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="124.5" customHeight="1">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -1153,10 +1202,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="124.5" customHeight="1">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -1167,10 +1216,10 @@
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="51" customHeight="1">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -1181,10 +1230,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="51" customHeight="1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -1195,10 +1244,10 @@
         <v>14</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="51" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>16</v>
       </c>
@@ -1206,13 +1255,13 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>80</v>
+        <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="51" customHeight="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -1223,10 +1272,10 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="70.5" customHeight="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -1237,10 +1286,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="51" customHeight="1">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -1251,10 +1300,10 @@
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="51" customHeight="1">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -1265,10 +1314,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="51" customHeight="1">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -1276,13 +1325,13 @@
         <v>20</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="72" customHeight="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -1293,10 +1342,10 @@
         <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51" customHeight="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>23</v>
       </c>
@@ -1304,13 +1353,13 @@
         <v>21</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="51" customHeight="1">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -1318,13 +1367,13 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>112</v>
+        <v>81</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="51" customHeight="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>25</v>
       </c>
@@ -1335,10 +1384,10 @@
         <v>24</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="51" customHeight="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>26</v>
       </c>
@@ -1349,10 +1398,10 @@
         <v>25</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="51" customHeight="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>27</v>
       </c>
@@ -1363,10 +1412,10 @@
         <v>26</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="51" customHeight="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>28</v>
       </c>
@@ -1374,13 +1423,13 @@
         <v>23</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="58.5" customHeight="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -1388,13 +1437,13 @@
         <v>27</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="51" customHeight="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -1402,13 +1451,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>103</v>
+        <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="51" customHeight="1">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -1416,13 +1465,13 @@
         <v>26</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>104</v>
+        <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="93" customHeight="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="123" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -1433,10 +1482,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="118.5" customHeight="1">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -1447,10 +1496,10 @@
         <v>29</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="61.5" customHeight="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>34</v>
       </c>
@@ -1461,10 +1510,10 @@
         <v>30</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="51" customHeight="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>35</v>
       </c>
@@ -1475,10 +1524,10 @@
         <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="153" customHeight="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>36</v>
       </c>
@@ -1489,10 +1538,10 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="153" customHeight="1">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -1503,10 +1552,10 @@
         <v>34</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="153" customHeight="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -1517,10 +1566,10 @@
         <v>35</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="153" customHeight="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>39</v>
       </c>
@@ -1531,10 +1580,10 @@
         <v>36</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="153" customHeight="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>40</v>
       </c>
@@ -1545,10 +1594,10 @@
         <v>37</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="153" customHeight="1">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>41</v>
       </c>
@@ -1559,10 +1608,10 @@
         <v>38</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="73.5" customHeight="1">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>42</v>
       </c>
@@ -1576,7 +1625,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="72.75" customHeight="1">
+    <row r="43" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>43</v>
       </c>
@@ -1587,10 +1636,10 @@
         <v>40</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="51" customHeight="1">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -1601,10 +1650,10 @@
         <v>41</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="73.5" customHeight="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -1615,10 +1664,10 @@
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="68.25" customHeight="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -1629,10 +1678,10 @@
         <v>43</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="51" customHeight="1">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -1643,10 +1692,10 @@
         <v>44</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="51" customHeight="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -1660,7 +1709,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="51" customHeight="1">
+    <row r="49" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -1674,7 +1723,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="51" customHeight="1">
+    <row r="50" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -1685,10 +1734,10 @@
         <v>47</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="51" customHeight="1">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>51</v>
       </c>
@@ -1699,10 +1748,10 @@
         <v>48</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="114" customHeight="1">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>52</v>
       </c>
@@ -1713,10 +1762,10 @@
         <v>49</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="51" customHeight="1">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>53</v>
       </c>
@@ -1727,10 +1776,10 @@
         <v>51</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="59.25" customHeight="1">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>54</v>
       </c>
@@ -1741,10 +1790,10 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="62.25" customHeight="1">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>55</v>
       </c>
@@ -1755,10 +1804,10 @@
         <v>14</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" ht="51" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>56</v>
       </c>
@@ -1769,10 +1818,10 @@
         <v>15</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" ht="64.5" customHeight="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>57</v>
       </c>
@@ -1783,10 +1832,10 @@
         <v>54</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="51" customHeight="1">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>58</v>
       </c>
@@ -1797,7 +1846,7 @@
         <v>31</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add more analysis functions
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Compiler-Semantic-Analyzer\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4872272A-274C-487D-9F29-C84A8A2A192E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E58B86C-701F-40DB-9824-3C2037A40FC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -296,22 +296,8 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve"> &lt;SB1&gt;.rT equals to &lt;SB2&gt;.rT: &lt;IS&gt;.rT = &lt;SB1&gt;.rT
-else: ERROR
-&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' 
-+ &lt;SB1&gt;.IR + 'goto L2' 
-+ 'L1:' + &lt;SB2&gt;.IR 
-+ 'L2:'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;VarDecl&gt;</t>
     <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
-&lt;SB&gt;.returnType = &lt;S&gt;.returnType
-&lt;SB&gt;.innerVarAmount = &lt;S&gt;.vA</t>
   </si>
   <si>
     <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
@@ -328,14 +314,6 @@
     <t>&lt;S&gt;.IR = &lt;VD&gt;.IR
 &lt;S&gt;.returnType = 'void'
 &lt;Stmt&gt;.innerVarAmount += 1 (default is 0)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;WS&gt;.returnType = &lt;SB&gt;.returnType
-&lt;WS&gt;.IR = 'L1:' + &lt;E&gt;.IR 
-+ 'if(&lt;E&gt;.val != 1) goto L2:'
-+ &lt;SB&gt;.IR + 'goto L1' 
-+ 'L2:'
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
   </si>
   <si>
     <t>&lt;Item&gt;.val = &lt;Factor&gt;.val
@@ -417,12 +395,6 @@
     <t>&lt;E&gt;.val = &lt;A&gt;.val
 &lt;E&gt;.valType = &lt;A&gt;.valType
 &lt;E&gt;.IR = &lt;A&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
-&lt;IF&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1:' + &lt;SB&gt;.IR + 'L1:'
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -636,6 +608,40 @@
 L3:'newTemp.valType = 'int'
 &lt;E1&gt;.val = newTemp
 &lt;E1&gt;.valType = newTemp.valType</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
+&lt;SB&gt;.returnType = &lt;S&gt;.returnType
+&lt;SB&gt;.innerVarAmount = &lt;S&gt;.vA
+pop &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;E&gt;.valType is not 'int': ERROR
+ &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;IS&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1 else L2:' 
++ 'L1:' + &lt;SB&gt;.IR + 
+'L2:'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;E&gt;.valType is not 'int': ERROR 
+&lt;SB1&gt;.rT equals to &lt;SB2&gt;.rT: &lt;IS&gt;.rT = &lt;SB1&gt;.rT
+else: ERROR
+&lt;IS&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1 else L2' 
++ 'L1:' + &lt;SB1&gt;.IR + 'goto L3' 
++ 'L2:' + &lt;SB2&gt;.IR 
++ 'L3:'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>if &lt;E&gt;.valType is not 'int': ERROR 
+ &lt;WS&gt;.returnType = &lt;SB&gt;.returnType
+&lt;WS&gt;.IR = 'L1:' + &lt;E&gt;.IR 
++ 'if(&lt;E&gt;.val == 1) goto L2 else L3:'
++ 'L2' + &lt;SB&gt;.IR + 'goto L1' 
++ 'L3:'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1024,8 +1030,8 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B35" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1132,7 +1138,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1146,7 +1152,7 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1160,7 +1166,7 @@
         <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1174,7 +1180,7 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1188,7 +1194,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1202,7 +1208,7 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1216,7 +1222,7 @@
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1230,7 +1236,7 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1272,7 +1278,7 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.2">
@@ -1286,7 +1292,7 @@
         <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1300,7 +1306,7 @@
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1314,10 +1320,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -1328,7 +1334,7 @@
         <v>66</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>82</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.2">
@@ -1342,7 +1348,7 @@
         <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1356,7 +1362,7 @@
         <v>65</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1367,10 +1373,10 @@
         <v>23</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1440,7 +1446,7 @@
         <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1454,7 +1460,7 @@
         <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1468,7 +1474,7 @@
         <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="123" customHeight="1" x14ac:dyDescent="0.2">
@@ -1482,7 +1488,7 @@
         <v>28</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>86</v>
+        <v>122</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1496,7 +1502,7 @@
         <v>29</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>80</v>
+        <v>121</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.2">
@@ -1510,7 +1516,7 @@
         <v>30</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>99</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1524,7 +1530,7 @@
         <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1538,7 +1544,7 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1552,7 +1558,7 @@
         <v>34</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1566,7 +1572,7 @@
         <v>35</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1580,7 +1586,7 @@
         <v>36</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1594,7 +1600,7 @@
         <v>37</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1608,7 +1614,7 @@
         <v>38</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.2">
@@ -1622,7 +1628,7 @@
         <v>39</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1636,7 +1642,7 @@
         <v>40</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1650,7 +1656,7 @@
         <v>41</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1664,7 +1670,7 @@
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1678,7 +1684,7 @@
         <v>43</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1692,7 +1698,7 @@
         <v>44</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
@@ -1734,7 +1740,7 @@
         <v>47</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1748,7 +1754,7 @@
         <v>48</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1762,7 +1768,7 @@
         <v>49</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1776,7 +1782,7 @@
         <v>51</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1790,7 +1796,7 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1832,7 +1838,7 @@
         <v>54</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -1846,7 +1852,7 @@
         <v>31</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
implemented some semantic analysis functions
</commit_message>
<xml_diff>
--- a/Assignments/Semantic.xlsx
+++ b/Assignments/Semantic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\Compiler-Semantic-Analyzer\Assignments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jake/Git/Compiler-Semantic-Analyzer/Assignments/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E58B86C-701F-40DB-9824-3C2037A40FC0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E124E839-5578-C54B-86D1-37E7243DE6F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="33600" windowHeight="19695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="33600" windowHeight="19700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="A Test Sheet" sheetId="1" r:id="rId1"/>
@@ -300,12 +300,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
-if &lt;S&gt; &lt;Stmts2&gt; rT equal: &lt;Stmts1&gt;.rT = &lt;Stmt&gt;.rT
-else: ERROR
-&lt;Stmts1&gt;.innerVarAmount = &lt;Stmt&gt;vA + &lt;Stmts2&gt;.vA</t>
-  </si>
-  <si>
     <t>&lt;Stmts&gt;.IR = &lt;S&gt;.IR
 &lt;Stmts&gt;.returnType = &lt;S&gt;.returnType
 &lt;Stmts&gt;.innerVarAmount = &lt;Stmt&gt;.innerVarAmount</t>
@@ -398,11 +392,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;RS&gt;.IR = 'ret ;'
-&lt;RS&gt;.returnType = 'void'</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>&lt;RS&gt;.IR = 'ret &lt;E&gt;.val ;'
 &lt;RS&gt;.returnType = &lt;E&gt;.varType</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -443,36 +432,6 @@
     <t>&lt;FP&gt;.paramType = &lt;PL&gt;.paramType 
 &lt;FP&gt;.paramName = &lt;PL&gt;.paramName
 &lt;FP&gt;.IR = &lt;PL&gt;.IR</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
-&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'void'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
-&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'float'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
-&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
-&lt;FD&gt;.returnType = 'int'
-&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
-&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
-insert into func symbol table
-push &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -611,13 +570,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
-&lt;SB&gt;.returnType = &lt;S&gt;.returnType
-&lt;SB&gt;.innerVarAmount = &lt;S&gt;.vA
-pop &lt;SB&gt;.innerVarAmount vars from var symbol table</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>if &lt;E&gt;.valType is not 'int': ERROR
  &lt;IS&gt;.returnType = &lt;SB&gt;.returnType
 &lt;IS&gt;.IR = &lt;E&gt;.IR + 'if (&lt;E&gt;.val != 1) goto L1 else L2:' 
@@ -644,12 +596,57 @@
 + 'L3:'</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>&lt;RS&gt;.IR = 'ret void'
+&lt;RS&gt;.returnType = 'void'</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;Stmts1&gt;.IR = &lt;Stmt&gt;.IR + &lt;Stmts2&gt;.IR
+if &lt;S&gt; &lt;Stmts2&gt; rT equal: &lt;Stmts1&gt;.rT = &lt;Stmt&gt;.rT
+else: ERROR
+&lt;Stmts1&gt;.innerVarAmount = &lt;Stmt&gt;.iVA + &lt;Stmts2&gt;.iVA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;SB&gt;.IR = &lt;S&gt;.IR
+&lt;SB&gt;.returnType = &lt;S&gt;.returnType
+pop &lt;S&gt;.innerVarAmount vars from var symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
+&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'void'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
+&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'int'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;FD&gt;.returnType != &lt;SB&gt;.rT: ERROR
+&lt;FD&gt;.IR = 'def func(' + &lt;FP&gt;.IR + ')' + &lt;SB&gt;.IR + '}'
+&lt;FD&gt;.returnType = 'float'
+&lt;FD&gt;.paramName = &lt;FP&gt;.paramName
+&lt;FD&gt;.paramType = &lt;FP&gt;.paramType
+insert into func symbol table</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1030,20 +1027,20 @@
   </sheetPr>
   <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C32" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="158" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="41.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="51.42578125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.1640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="41.83203125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="51.5" style="2" customWidth="1"/>
+    <col min="4" max="4" width="54.83203125" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="51" customHeight="1">
       <c r="A1" s="2">
         <v>1</v>
       </c>
@@ -1057,7 +1054,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="51" customHeight="1">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -1071,7 +1068,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="51" customHeight="1">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -1085,7 +1082,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="51" customHeight="1">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -1099,7 +1096,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="51" customHeight="1">
       <c r="A5" s="2">
         <v>5</v>
       </c>
@@ -1113,7 +1110,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="51" customHeight="1">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -1127,7 +1124,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="51" customHeight="1">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -1138,10 +1135,10 @@
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="64.5" customHeight="1">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -1152,10 +1149,10 @@
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="51" customHeight="1">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -1166,10 +1163,10 @@
         <v>57</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="74.25" customHeight="1">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -1180,10 +1177,10 @@
         <v>8</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="124.5" customHeight="1">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -1194,10 +1191,10 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="124.5" customHeight="1">
       <c r="A12" s="2">
         <v>12</v>
       </c>
@@ -1208,10 +1205,10 @@
         <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="124.5" customHeight="1">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -1222,10 +1219,10 @@
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="51" customHeight="1">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -1236,10 +1233,10 @@
         <v>13</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51" customHeight="1">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -1253,7 +1250,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="51" customHeight="1">
       <c r="A16" s="2">
         <v>16</v>
       </c>
@@ -1267,7 +1264,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="51" customHeight="1">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -1278,10 +1275,10 @@
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="78" customHeight="1" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="78" customHeight="1">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -1292,10 +1289,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51" customHeight="1">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -1306,10 +1303,10 @@
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="51" customHeight="1">
       <c r="A20" s="2">
         <v>20</v>
       </c>
@@ -1320,10 +1317,10 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="60.75" customHeight="1">
       <c r="A21" s="2">
         <v>21</v>
       </c>
@@ -1337,7 +1334,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="72" customHeight="1">
       <c r="A22" s="2">
         <v>22</v>
       </c>
@@ -1348,10 +1345,10 @@
         <v>22</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="51" customHeight="1">
       <c r="A23" s="2">
         <v>23</v>
       </c>
@@ -1362,10 +1359,10 @@
         <v>65</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="51" customHeight="1">
       <c r="A24" s="2">
         <v>24</v>
       </c>
@@ -1376,10 +1373,10 @@
         <v>80</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="51" customHeight="1">
       <c r="A25" s="2">
         <v>25</v>
       </c>
@@ -1393,7 +1390,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="51" customHeight="1">
       <c r="A26" s="2">
         <v>26</v>
       </c>
@@ -1407,7 +1404,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="51" customHeight="1">
       <c r="A27" s="2">
         <v>27</v>
       </c>
@@ -1421,7 +1418,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="51" customHeight="1">
       <c r="A28" s="2">
         <v>28</v>
       </c>
@@ -1435,7 +1432,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="58.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="58.5" customHeight="1">
       <c r="A29" s="2">
         <v>29</v>
       </c>
@@ -1446,10 +1443,10 @@
         <v>60</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="51" customHeight="1">
       <c r="A30" s="2">
         <v>30</v>
       </c>
@@ -1460,10 +1457,10 @@
         <v>74</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="51" customHeight="1">
       <c r="A31" s="2">
         <v>31</v>
       </c>
@@ -1474,10 +1471,10 @@
         <v>75</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="123" customHeight="1" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="123" customHeight="1">
       <c r="A32" s="2">
         <v>32</v>
       </c>
@@ -1488,10 +1485,10 @@
         <v>28</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="118.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="118.5" customHeight="1">
       <c r="A33" s="2">
         <v>33</v>
       </c>
@@ -1502,10 +1499,10 @@
         <v>29</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="93" customHeight="1" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="93" customHeight="1">
       <c r="A34" s="2">
         <v>34</v>
       </c>
@@ -1516,10 +1513,10 @@
         <v>30</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="51" customHeight="1">
       <c r="A35" s="2">
         <v>35</v>
       </c>
@@ -1530,10 +1527,10 @@
         <v>32</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="176.25" customHeight="1">
       <c r="A36" s="2">
         <v>36</v>
       </c>
@@ -1544,10 +1541,10 @@
         <v>33</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="176.25" customHeight="1">
       <c r="A37" s="2">
         <v>37</v>
       </c>
@@ -1558,10 +1555,10 @@
         <v>34</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="176.25" customHeight="1">
       <c r="A38" s="2">
         <v>38</v>
       </c>
@@ -1572,10 +1569,10 @@
         <v>35</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="176.25" customHeight="1">
       <c r="A39" s="2">
         <v>39</v>
       </c>
@@ -1586,10 +1583,10 @@
         <v>36</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="176.25" customHeight="1">
       <c r="A40" s="2">
         <v>40</v>
       </c>
@@ -1600,10 +1597,10 @@
         <v>37</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="176.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="176.25" customHeight="1">
       <c r="A41" s="2">
         <v>41</v>
       </c>
@@ -1614,10 +1611,10 @@
         <v>38</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="87" customHeight="1" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="87" customHeight="1">
       <c r="A42" s="2">
         <v>42</v>
       </c>
@@ -1628,10 +1625,10 @@
         <v>39</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="93.75" customHeight="1">
       <c r="A43" s="2">
         <v>43</v>
       </c>
@@ -1642,10 +1639,10 @@
         <v>40</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="51" customHeight="1">
       <c r="A44" s="2">
         <v>44</v>
       </c>
@@ -1656,10 +1653,10 @@
         <v>41</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="88.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="88.5" customHeight="1">
       <c r="A45" s="2">
         <v>45</v>
       </c>
@@ -1670,10 +1667,10 @@
         <v>42</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="96.75" customHeight="1">
       <c r="A46" s="2">
         <v>46</v>
       </c>
@@ -1684,10 +1681,10 @@
         <v>43</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="51" customHeight="1">
       <c r="A47" s="2">
         <v>47</v>
       </c>
@@ -1698,10 +1695,10 @@
         <v>44</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="51" customHeight="1">
       <c r="A48" s="2">
         <v>48</v>
       </c>
@@ -1715,7 +1712,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="51" customHeight="1">
       <c r="A49" s="2">
         <v>49</v>
       </c>
@@ -1729,7 +1726,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="51" customHeight="1">
       <c r="A50" s="2">
         <v>50</v>
       </c>
@@ -1740,10 +1737,10 @@
         <v>47</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="75" customHeight="1">
       <c r="A51" s="2">
         <v>51</v>
       </c>
@@ -1754,10 +1751,10 @@
         <v>48</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="134.25" customHeight="1">
       <c r="A52" s="2">
         <v>52</v>
       </c>
@@ -1768,10 +1765,10 @@
         <v>49</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="134.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="134.25" customHeight="1">
       <c r="A53" s="2">
         <v>53</v>
       </c>
@@ -1782,10 +1779,10 @@
         <v>51</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="59.25" customHeight="1">
       <c r="A54" s="2">
         <v>54</v>
       </c>
@@ -1796,10 +1793,10 @@
         <v>53</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="62.25" customHeight="1">
       <c r="A55" s="2">
         <v>55</v>
       </c>
@@ -1813,7 +1810,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="51" customHeight="1">
       <c r="A56" s="2">
         <v>56</v>
       </c>
@@ -1827,7 +1824,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="79.5" customHeight="1">
       <c r="A57" s="2">
         <v>57</v>
       </c>
@@ -1838,10 +1835,10 @@
         <v>54</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="74.25" customHeight="1" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="74.25" customHeight="1">
       <c r="A58" s="2">
         <v>58</v>
       </c>
@@ -1852,7 +1849,7 @@
         <v>31</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>